<commit_message>
Phs accession, Study and Gender filter test cases
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Gender-Male.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Gender-Male.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\CDS Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7014FE-9120-4217-AC39-BADE3F9ACBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA449BC4-7B51-49A5-B979-95606EE1D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,38 @@
     <t>FilesTab</t>
   </si>
   <si>
+    <t>TC01_CDS_Filter_Gender-Male_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_CDS_Filter_Gender-Male_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE p.gender in ["Male"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+WITH p, s, collect(distinct samp.sample_id) as samp
+RETURN   
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+ coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ ORDER By p.participant_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
+WHERE p.gender in ["Male"]
+WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
+RETURN  
+ coalesce(samp.sample_id, '') as `Sample ID`,
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER By samp.sample_id LIMIT 100</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;--(p:participant)
 WHERE p.gender in ["Male"]
 OPTIONAL MATCH (p)&lt;--(samp:sample)
@@ -84,38 +116,6 @@
     count(distinct p) AS Participants,
     count(distinct samp) AS Samples,
     count(distinct f) AS `Files`</t>
-  </si>
-  <si>
-    <t>TC01_CDS_Filter_Gender-Male_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_CDS_Filter_Gender-Male_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE p.gender in ["Male"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN   
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(apoc.text.join(samp, ','), '') as `Samples`
- ORDER By p.participant_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
-WHERE p.gender in ["Male"]
-WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
-RETURN  
- coalesce(samp.sample_id, '') as `Sample ID`,
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -497,19 +497,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="63.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -526,62 +526,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="218.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="249" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>